<commit_message>
copy diageous-sand2 to prod
</commit_message>
<xml_diff>
--- a/Projects/DIAGEOUS/Data/Template.xlsx
+++ b/Projects/DIAGEOUS/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="national - on_trade" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="39">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -80,28 +80,25 @@
     <t xml:space="preserve">1. Main Shelf, 3. Cold Box Shelf, 1. Spirits Main Shelf – OLD, 2. Behind the Counter Shelf</t>
   </si>
   <si>
+    <t xml:space="preserve">Previous Weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch Date</t>
+  </si>
+  <si>
     <t xml:space="preserve">Display Brand</t>
   </si>
   <si>
+    <t xml:space="preserve">Shelf Placement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MSRP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Back Bar</t>
+  </si>
+  <si>
     <t xml:space="preserve">1. Main Menu, 2. Features Menu, 3. Spirits List Menu, 4. Bottle List Menu, 5. After Dinner / Dessert Menu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Back Bar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Previous Weight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Switch Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Floor Display, 2. End Cap Display, 3. Rack Display, 4. One Case Bin Display, 5. Standalone Barrel Display, 6. Lock Box Display, 2. Spirits Displays - OLD, Craftswomen Display</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shelf Placement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MSRP</t>
   </si>
   <si>
     <t xml:space="preserve">number group</t>
@@ -375,7 +372,7 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.9473684210526"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="67.5910931174089"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -471,9 +468,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.0283400809717"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.3117408906883"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.7368421052632"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="6" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.46153846153846"/>
   </cols>
@@ -562,17 +559,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.0283400809717"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.3076923076923"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.7368421052632"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="6" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.46153846153846"/>
   </cols>
@@ -593,27 +590,39 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="F1" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.65</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="G2" s="7" t="n">
+        <v>43647</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>6</v>
@@ -621,11 +630,110 @@
       <c r="C3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="4" t="n">
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <f aca="false">0.72*0.35</f>
+        <v>0.252</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>0.0875</v>
+      </c>
+      <c r="G3" s="7" t="n">
+        <v>43647</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4" t="n">
         <v>0.25</v>
       </c>
-      <c r="E3" s="4" t="n">
-        <v>0</v>
+      <c r="E4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>0.0875</v>
+      </c>
+      <c r="G4" s="7" t="n">
+        <v>43647</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <f aca="false">0.5*0.28*0.35</f>
+        <v>0.049</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0.0875</v>
+      </c>
+      <c r="G5" s="7" t="n">
+        <v>43647</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="4" t="n">
+        <f aca="false">0.5*0.28*0.35</f>
+        <v>0.049</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>0.0875</v>
+      </c>
+      <c r="G6" s="7" t="n">
+        <v>43647</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="7" t="n">
+        <v>43647</v>
       </c>
     </row>
   </sheetData>
@@ -644,17 +752,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.246963562753"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="56.5587044534413"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="56.9878542510121"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -675,21 +783,55 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="4" t="n">
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="4" t="n">
         <v>0.25</v>
       </c>
-      <c r="E2" s="4" t="n">
-        <v>0</v>
+      <c r="E4" s="4" t="n">
+        <v>0.35</v>
       </c>
     </row>
   </sheetData>
@@ -711,14 +853,14 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="84.5182186234818"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="85.2672064777328"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -747,7 +889,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>8</v>
@@ -764,7 +906,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>8</v>
@@ -781,7 +923,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D4" s="4" t="n">
         <v>0.25</v>
@@ -808,19 +950,19 @@
   </sheetPr>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.0283400809717"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.3117408906883"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.7368421052632"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="6" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.2834008097166"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.46153846153846"/>
   </cols>
   <sheetData>
@@ -841,10 +983,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -872,13 +1014,13 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>8</v>
@@ -902,7 +1044,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D4" s="4" t="n">
         <v>0.25</v>
@@ -943,7 +1085,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>6</v>
@@ -967,7 +1109,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
@@ -1011,16 +1153,16 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.5303643724696"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1028,7 +1170,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1036,7 +1178,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1044,7 +1186,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1052,7 +1194,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1060,7 +1202,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1068,7 +1210,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1076,7 +1218,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1136,77 +1278,77 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>35</v>
-      </c>
       <c r="C2" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>36</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E6" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F7" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>